<commit_message>
i added file permission checker. now if you forgot to close the file, you will obtain normal message instead of error.
</commit_message>
<xml_diff>
--- a/capture.xlsx
+++ b/capture.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1536,6 +1539,198 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr"/>
+      <c r="B43" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">suspend                  </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>to officially stop something or somebody for a time/to hang something from something else</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Production has been suspended while safety checks are carried out/A lamp was suspended from the ceiling.</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr"/>
+      <c r="B44" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sweep                    </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>to clean a room/push something with a lot of force</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>to sweep the floor/ the little boat was swept out to sea</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr"/>
+      <c r="B45" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tackle                   </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>to make a determined effort to deal with a difficult problem or situation</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Firefighters tackled a blaze in a garage last night</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr"/>
+      <c r="B46" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tale </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>a story</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>The story is a classic tale of love and betrayal.</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr"/>
+      <c r="B47" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tension                  </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>a situation in which people do not trust each other, or feel unfriendly</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Family tensions and conflicts may lead to violence</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr"/>
+      <c r="B48" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thorough                 </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>done completely; with great attention to detail</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>a thorough knowledge of the subject</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr"/>
+      <c r="B49" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tissue                   </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>a piece of soft paper, used especially as a handkerchief</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>a box of tissues</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr"/>
+      <c r="B50" s="3" t="n">
+        <v>44924</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trace       </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>to find or discover somebody/something by looking carefully for them/it  OR / gentally touch</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>We finally traced him to an address in Chicago /She lightly traced the outline of his face with her finger</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adjusted a bug with saving file, now, should be nice, tho
</commit_message>
<xml_diff>
--- a/capture.xlsx
+++ b/capture.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="3">
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="4">
@@ -555,10 +555,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="5">
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="6">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="7">
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="8">
@@ -671,10 +671,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="9">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="10">
@@ -729,10 +729,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="11">
@@ -758,10 +758,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="12">
@@ -787,10 +787,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="13">
@@ -816,10 +816,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="14">
@@ -845,10 +845,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="15">
@@ -874,10 +874,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="16">
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="17">
@@ -932,10 +932,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="18">
@@ -961,10 +961,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="19">
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="20">
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="21">
@@ -1048,10 +1048,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="22">
@@ -1077,10 +1077,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="23">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="24">
@@ -1136,10 +1136,10 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="25">
@@ -1165,10 +1165,10 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="26">
@@ -1194,10 +1194,10 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="27">
@@ -1223,10 +1223,10 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="28">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="29">
@@ -1281,10 +1281,10 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="30">
@@ -1310,10 +1310,10 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="31">
@@ -1339,10 +1339,10 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="32">
@@ -1368,10 +1368,10 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="33">
@@ -1397,10 +1397,10 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="34">
@@ -1426,10 +1426,10 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="35">
@@ -1455,10 +1455,10 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="36">
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="37">
@@ -1513,10 +1513,10 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="38">
@@ -1542,10 +1542,10 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="39">
@@ -1571,10 +1571,10 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="40">
@@ -1600,10 +1600,10 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="41">
@@ -1629,10 +1629,10 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="42">
@@ -1658,10 +1658,10 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="43">
@@ -1685,10 +1685,10 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="44">
@@ -1712,10 +1712,10 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="45">
@@ -1739,10 +1739,10 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="46">
@@ -1766,10 +1766,10 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="47">
@@ -1793,10 +1793,10 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="48">
@@ -1820,10 +1820,10 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="49">
@@ -1847,10 +1847,10 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="50">
@@ -1874,10 +1874,10 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="51">
@@ -1901,10 +1901,10 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="52">
@@ -1928,10 +1928,10 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="53">
@@ -1955,10 +1955,10 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="54">
@@ -1982,10 +1982,10 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="55">
@@ -2009,10 +2009,10 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="56">
@@ -2036,10 +2036,10 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="57">
@@ -2063,10 +2063,10 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="58">
@@ -2090,10 +2090,10 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="59">
@@ -2117,10 +2117,10 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>44926</v>
+        <v>44928</v>
       </c>
     </row>
     <row r="60">
@@ -2144,10 +2144,253 @@
         </is>
       </c>
       <c r="F60" t="n">
+        <v>3</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr"/>
+      <c r="B61" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">venue                    </t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>the place where a public event or meeting happens:</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>The hotel is an ideal venue for conferences and business meetings.</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
         <v>1</v>
       </c>
-      <c r="G60" s="2" t="n">
+      <c r="G61" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr"/>
+      <c r="B62" s="2" t="n">
         <v>44926</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wage                     </t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>a regular amount of money that you earn, usually every week or every month, for work or services</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>a weekly wage of £300</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr"/>
+      <c r="B63" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wander                   </t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>to walk slowly around or to a place, often without any particular sense of purpose or direction</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>We wandered back towards the car.</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr"/>
+      <c r="B64" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wealth                   </t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>a large amount of money, property, etc. that a person or country owns</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>the desire to gain wealth and power</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr"/>
+      <c r="B65" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">welfare                  </t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>the general health, happiness and safety of a person, an animal or a group</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>We are concerned about the child's welfare.</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr"/>
+      <c r="B66" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wheat                    </t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>a plant whose yellowish-brown grain is used for making flour, or the grain itself:</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>wheat flour</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr"/>
+      <c r="B67" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wound                    </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>an injury to part of the body, especially one in which a hole is made in the skin using a weapon</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>a bullet/knife/shrapnel wound</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr"/>
+      <c r="B68" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wrist                    </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>the joint between the hand and the arm</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>She's broken her wrist.</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>44928</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr"/>
+      <c r="B69" s="2" t="n">
+        <v>44926</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">abolish     </t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>to end an activity or custom officially:</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>I think bullfighting should be abolished.</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="2" t="n">
+        <v>44928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did some changes to educational system.
</commit_message>
<xml_diff>
--- a/capture.xlsx
+++ b/capture.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2690,6 +2690,304 @@
         <v>44930</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr"/>
+      <c r="B81" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>stir</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>mix / to move, or to make something move, slightly / to make somebody excited or make them feel something strongly</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>She stirred her tea. / She heard the baby stir in the next room. / It's a book that really stirs the imagination</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr"/>
+      <c r="B82" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>preservation</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>the act of keeping something in its original state or in good condition</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>building/environmental/food preservation</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr"/>
+      <c r="B83" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>spouse</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>a husband or wife</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Fill in your spouse’s name here.</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr"/>
+      <c r="B84" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>utility</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>a service provided for the public, for example an electricity, water or gas supply</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>a privatized electricity utility</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr"/>
+      <c r="B85" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>verse</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>a group of lines that form a unit in a poem or song</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+a hymn with six verses</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr"/>
+      <c r="B86" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>venture</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>a business project or activity, especially one that involves taking risks</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>A disastrous business venture lost him thousands of dollars.</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr"/>
+      <c r="B87" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>contractor</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>a person or company that has a contract to do work or provide goods or services for another company</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>a building/roofing/electrical contractor</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr"/>
+      <c r="B88" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>weave</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>c1[transitive, intransitive]to make cloth, a carpet, a basket, etc. by crossing threads or narrow pieces of material across, over and under each other by hand or on a machine called a loom</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Most spiders weave webs that are almost invisible.</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr"/>
+      <c r="B89" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>refusal</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>an act of saying or showing that you will not do, give or accept something</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>the refusal of a request/an invitation/an offer</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr"/>
+      <c r="B90" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>interfere</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>to get involved in and try to influence a situation that should not really involve you, in a way that annoys other people</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>I wish my mother would stop interfering and let me make my own decisions.</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr"/>
+      <c r="B91" s="2" t="n">
+        <v>44930</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>chronic</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>c1lasting for a long time; difficult to cure</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>chronic bronchitis/arthritis/asthma</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" s="2" t="n">
+        <v>44929</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
silly bugs were destroyed
</commit_message>
<xml_diff>
--- a/capture.xlsx
+++ b/capture.xlsx
@@ -510,13 +510,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -545,13 +545,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -580,13 +580,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -615,13 +615,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -650,13 +650,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>44939</v>
+        <v>44954</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -685,13 +685,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -720,13 +720,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -755,13 +755,13 @@
         <v>5</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -790,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -825,13 +825,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -860,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -895,13 +895,13 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -930,13 +930,13 @@
         <v>5</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -965,13 +965,13 @@
         <v>5</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1000,13 +1000,13 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1035,13 +1035,13 @@
         <v>5</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1070,13 +1070,13 @@
         <v>5</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1105,13 +1105,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1140,13 +1140,13 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H20" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1175,13 +1175,13 @@
         <v>5</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H21" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -1210,13 +1210,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H22" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1246,13 +1246,13 @@
         <v>5</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H23" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1281,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H24" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1316,13 +1316,13 @@
         <v>5</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H25" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1351,13 +1351,13 @@
         <v>5</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H26" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1386,13 +1386,13 @@
         <v>5</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H27" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1421,13 +1421,13 @@
         <v>5</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1456,13 +1456,13 @@
         <v>5</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H29" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1491,13 +1491,13 @@
         <v>5</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H30" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1526,13 +1526,13 @@
         <v>5</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H31" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1561,13 +1561,13 @@
         <v>5</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1596,13 +1596,13 @@
         <v>5</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H33" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -1631,13 +1631,13 @@
         <v>5</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1666,13 +1666,13 @@
         <v>5</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H35" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1701,13 +1701,13 @@
         <v>5</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H36" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -1736,13 +1736,13 @@
         <v>5</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>44933</v>
+        <v>44954</v>
       </c>
       <c r="H37" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1771,13 +1771,13 @@
         <v>5</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H38" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1806,13 +1806,13 @@
         <v>5</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H39" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -1841,13 +1841,13 @@
         <v>5</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H40" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -1876,13 +1876,13 @@
         <v>5</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H41" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
@@ -1911,13 +1911,13 @@
         <v>5</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H42" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -1944,13 +1944,13 @@
         <v>5</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H43" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -1977,13 +1977,13 @@
         <v>5</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>44937</v>
+        <v>44954</v>
       </c>
       <c r="H44" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
@@ -2010,13 +2010,13 @@
         <v>5</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H45" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -2043,13 +2043,13 @@
         <v>5</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H46" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -2076,13 +2076,13 @@
         <v>5</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H47" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2109,13 +2109,13 @@
         <v>5</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H48" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
@@ -2142,13 +2142,13 @@
         <v>5</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H49" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -2175,13 +2175,13 @@
         <v>5</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H50" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -2208,13 +2208,13 @@
         <v>5</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H51" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -2241,13 +2241,13 @@
         <v>5</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H52" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2274,13 +2274,13 @@
         <v>5</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H53" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2307,13 +2307,13 @@
         <v>5</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H54" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -2340,13 +2340,13 @@
         <v>5</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H55" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -2373,13 +2373,13 @@
         <v>5</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H56" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -2406,13 +2406,13 @@
         <v>5</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H57" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -2439,13 +2439,13 @@
         <v>5</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H58" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2472,13 +2472,13 @@
         <v>5</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>44938</v>
+        <v>44954</v>
       </c>
       <c r="H59" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2505,13 +2505,13 @@
         <v>5</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H60" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2538,13 +2538,13 @@
         <v>5</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H61" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
@@ -2571,13 +2571,13 @@
         <v>5</v>
       </c>
       <c r="G62" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H62" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -2604,13 +2604,13 @@
         <v>5</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H63" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64">
@@ -2637,13 +2637,13 @@
         <v>5</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H64" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2670,13 +2670,13 @@
         <v>5</v>
       </c>
       <c r="G65" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H65" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2703,13 +2703,13 @@
         <v>5</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H66" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2736,13 +2736,13 @@
         <v>5</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H67" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -2769,13 +2769,13 @@
         <v>5</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H68" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I68" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -2802,13 +2802,13 @@
         <v>5</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H69" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
@@ -2835,13 +2835,13 @@
         <v>5</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H70" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2868,13 +2868,13 @@
         <v>5</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H71" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
@@ -2901,13 +2901,13 @@
         <v>5</v>
       </c>
       <c r="G72" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H72" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2934,13 +2934,13 @@
         <v>5</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H73" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I73" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -2967,13 +2967,13 @@
         <v>5</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H74" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75">
@@ -3000,13 +3000,13 @@
         <v>5</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H75" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I75" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -3033,13 +3033,13 @@
         <v>5</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H76" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3066,13 +3066,13 @@
         <v>5</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>44938</v>
+        <v>44954</v>
       </c>
       <c r="H77" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -3099,13 +3099,13 @@
         <v>5</v>
       </c>
       <c r="G78" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H78" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -3132,13 +3132,13 @@
         <v>5</v>
       </c>
       <c r="G79" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H79" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
@@ -3165,13 +3165,13 @@
         <v>5</v>
       </c>
       <c r="G80" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H80" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3198,13 +3198,13 @@
         <v>5</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H81" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3231,13 +3231,13 @@
         <v>5</v>
       </c>
       <c r="G82" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H82" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3264,13 +3264,13 @@
         <v>5</v>
       </c>
       <c r="G83" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H83" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3297,13 +3297,13 @@
         <v>5</v>
       </c>
       <c r="G84" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H84" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I84" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3331,13 +3331,13 @@
         <v>5</v>
       </c>
       <c r="G85" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H85" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -3364,13 +3364,13 @@
         <v>5</v>
       </c>
       <c r="G86" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H86" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3397,13 +3397,13 @@
         <v>5</v>
       </c>
       <c r="G87" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H87" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -3430,13 +3430,13 @@
         <v>5</v>
       </c>
       <c r="G88" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H88" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3463,13 +3463,13 @@
         <v>5</v>
       </c>
       <c r="G89" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H89" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -3496,13 +3496,13 @@
         <v>5</v>
       </c>
       <c r="G90" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H90" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I90" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -3529,13 +3529,13 @@
         <v>5</v>
       </c>
       <c r="G91" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H91" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3562,13 +3562,13 @@
         <v>5</v>
       </c>
       <c r="G92" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H92" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93">
@@ -3595,13 +3595,13 @@
         <v>5</v>
       </c>
       <c r="G93" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H93" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94">
@@ -3628,13 +3628,13 @@
         <v>5</v>
       </c>
       <c r="G94" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H94" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95">
@@ -3661,13 +3661,13 @@
         <v>5</v>
       </c>
       <c r="G95" s="2" t="n">
-        <v>44937</v>
+        <v>44954</v>
       </c>
       <c r="H95" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -3694,13 +3694,13 @@
         <v>5</v>
       </c>
       <c r="G96" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H96" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I96" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97">
@@ -3727,13 +3727,13 @@
         <v>5</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H97" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -3760,13 +3760,13 @@
         <v>5</v>
       </c>
       <c r="G98" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H98" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I98" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99">
@@ -3793,13 +3793,13 @@
         <v>5</v>
       </c>
       <c r="G99" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H99" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
@@ -3826,13 +3826,13 @@
         <v>5</v>
       </c>
       <c r="G100" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H100" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3859,13 +3859,13 @@
         <v>5</v>
       </c>
       <c r="G101" s="2" t="n">
-        <v>44938</v>
+        <v>44954</v>
       </c>
       <c r="H101" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -3892,13 +3892,13 @@
         <v>5</v>
       </c>
       <c r="G102" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H102" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -3925,13 +3925,13 @@
         <v>5</v>
       </c>
       <c r="G103" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H103" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -3958,13 +3958,13 @@
         <v>5</v>
       </c>
       <c r="G104" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H104" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I104" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
@@ -3991,13 +3991,13 @@
         <v>5</v>
       </c>
       <c r="G105" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H105" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -4024,13 +4024,13 @@
         <v>5</v>
       </c>
       <c r="G106" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H106" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I106" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
@@ -4057,13 +4057,13 @@
         <v>5</v>
       </c>
       <c r="G107" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H107" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108">
@@ -4090,13 +4090,13 @@
         <v>5</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H108" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I108" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -4123,13 +4123,13 @@
         <v>5</v>
       </c>
       <c r="G109" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H109" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I109" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -4156,13 +4156,13 @@
         <v>5</v>
       </c>
       <c r="G110" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H110" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I110" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
@@ -4189,13 +4189,13 @@
         <v>5</v>
       </c>
       <c r="G111" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H111" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4222,13 +4222,13 @@
         <v>5</v>
       </c>
       <c r="G112" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H112" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I112" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
@@ -4255,13 +4255,13 @@
         <v>5</v>
       </c>
       <c r="G113" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H113" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -4288,13 +4288,13 @@
         <v>5</v>
       </c>
       <c r="G114" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H114" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I114" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -4321,13 +4321,13 @@
         <v>5</v>
       </c>
       <c r="G115" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H115" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -4354,13 +4354,13 @@
         <v>5</v>
       </c>
       <c r="G116" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H116" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117">
@@ -4387,13 +4387,13 @@
         <v>5</v>
       </c>
       <c r="G117" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H117" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I117" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
@@ -4420,13 +4420,13 @@
         <v>5</v>
       </c>
       <c r="G118" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H118" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -4453,13 +4453,13 @@
         <v>5</v>
       </c>
       <c r="G119" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H119" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -4486,13 +4486,13 @@
         <v>5</v>
       </c>
       <c r="G120" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H120" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I120" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121">
@@ -4519,13 +4519,13 @@
         <v>5</v>
       </c>
       <c r="G121" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H121" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I121" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122">
@@ -4552,13 +4552,13 @@
         <v>5</v>
       </c>
       <c r="G122" s="2" t="n">
-        <v>44940</v>
+        <v>44954</v>
       </c>
       <c r="H122" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I122" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123">
@@ -4585,13 +4585,13 @@
         <v>5</v>
       </c>
       <c r="G123" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H123" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
@@ -4618,13 +4618,13 @@
         <v>5</v>
       </c>
       <c r="G124" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H124" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I124" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -4651,13 +4651,13 @@
         <v>5</v>
       </c>
       <c r="G125" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H125" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126">
@@ -4684,13 +4684,13 @@
         <v>5</v>
       </c>
       <c r="G126" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H126" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I126" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127">
@@ -4717,13 +4717,13 @@
         <v>5</v>
       </c>
       <c r="G127" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H127" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -4750,13 +4750,13 @@
         <v>5</v>
       </c>
       <c r="G128" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H128" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129">
@@ -4783,13 +4783,13 @@
         <v>5</v>
       </c>
       <c r="G129" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H129" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I129" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
@@ -4816,13 +4816,13 @@
         <v>5</v>
       </c>
       <c r="G130" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H130" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I130" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
@@ -4849,13 +4849,13 @@
         <v>5</v>
       </c>
       <c r="G131" s="2" t="n">
-        <v>44941</v>
+        <v>44954</v>
       </c>
       <c r="H131" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -4882,13 +4882,13 @@
         <v>5</v>
       </c>
       <c r="G132" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H132" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -4915,13 +4915,13 @@
         <v>5</v>
       </c>
       <c r="G133" s="2" t="n">
-        <v>44948</v>
+        <v>44954</v>
       </c>
       <c r="H133" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134">
@@ -4948,13 +4948,13 @@
         <v>5</v>
       </c>
       <c r="G134" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H134" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I134" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
@@ -4981,13 +4981,13 @@
         <v>5</v>
       </c>
       <c r="G135" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H135" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I135" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
@@ -5014,13 +5014,13 @@
         <v>5</v>
       </c>
       <c r="G136" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H136" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I136" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137">
@@ -5047,13 +5047,13 @@
         <v>5</v>
       </c>
       <c r="G137" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H137" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -5080,13 +5080,13 @@
         <v>5</v>
       </c>
       <c r="G138" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H138" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I138" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139">
@@ -5113,13 +5113,13 @@
         <v>5</v>
       </c>
       <c r="G139" s="2" t="n">
-        <v>44943</v>
+        <v>44954</v>
       </c>
       <c r="H139" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I139" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140">
@@ -5146,13 +5146,13 @@
         <v>5</v>
       </c>
       <c r="G140" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H140" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
@@ -5179,13 +5179,13 @@
         <v>5</v>
       </c>
       <c r="G141" s="2" t="n">
-        <v>44943</v>
+        <v>44954</v>
       </c>
       <c r="H141" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I141" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
@@ -5212,13 +5212,13 @@
         <v>5</v>
       </c>
       <c r="G142" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H142" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I142" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
@@ -5245,13 +5245,13 @@
         <v>5</v>
       </c>
       <c r="G143" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H143" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I143" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144">
@@ -5278,13 +5278,13 @@
         <v>5</v>
       </c>
       <c r="G144" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H144" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -5311,13 +5311,13 @@
         <v>5</v>
       </c>
       <c r="G145" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H145" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I145" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146">
@@ -5344,13 +5344,13 @@
         <v>5</v>
       </c>
       <c r="G146" s="2" t="n">
-        <v>44942</v>
+        <v>44954</v>
       </c>
       <c r="H146" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -5377,13 +5377,13 @@
         <v>5</v>
       </c>
       <c r="G147" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H147" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -5410,13 +5410,13 @@
         <v>5</v>
       </c>
       <c r="G148" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H148" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I148" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
@@ -5443,13 +5443,13 @@
         <v>5</v>
       </c>
       <c r="G149" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H149" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -5476,13 +5476,13 @@
         <v>5</v>
       </c>
       <c r="G150" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H150" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -5509,13 +5509,13 @@
         <v>5</v>
       </c>
       <c r="G151" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H151" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
@@ -5542,13 +5542,13 @@
         <v>5</v>
       </c>
       <c r="G152" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H152" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I152" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -5575,13 +5575,13 @@
         <v>5</v>
       </c>
       <c r="G153" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H153" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I153" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154">
@@ -5608,13 +5608,13 @@
         <v>5</v>
       </c>
       <c r="G154" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H154" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -5641,13 +5641,13 @@
         <v>5</v>
       </c>
       <c r="G155" s="2" t="n">
-        <v>44945</v>
+        <v>44954</v>
       </c>
       <c r="H155" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I155" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -5675,13 +5675,13 @@
         <v>5</v>
       </c>
       <c r="G156" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H156" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -5708,13 +5708,13 @@
         <v>5</v>
       </c>
       <c r="G157" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H157" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I157" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -5741,13 +5741,13 @@
         <v>5</v>
       </c>
       <c r="G158" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H158" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I158" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159">
@@ -5774,13 +5774,13 @@
         <v>5</v>
       </c>
       <c r="G159" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H159" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -5807,13 +5807,13 @@
         <v>5</v>
       </c>
       <c r="G160" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H160" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -5840,13 +5840,13 @@
         <v>5</v>
       </c>
       <c r="G161" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H161" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I161" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162">
@@ -5873,13 +5873,13 @@
         <v>5</v>
       </c>
       <c r="G162" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H162" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I162" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -5906,13 +5906,13 @@
         <v>5</v>
       </c>
       <c r="G163" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H163" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I163" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
@@ -5939,13 +5939,13 @@
         <v>5</v>
       </c>
       <c r="G164" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H164" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I164" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -5972,13 +5972,13 @@
         <v>5</v>
       </c>
       <c r="G165" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H165" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I165" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166">
@@ -6005,13 +6005,13 @@
         <v>5</v>
       </c>
       <c r="G166" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H166" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -6038,13 +6038,13 @@
         <v>5</v>
       </c>
       <c r="G167" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H167" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -6071,13 +6071,13 @@
         <v>5</v>
       </c>
       <c r="G168" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H168" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I168" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -6104,13 +6104,13 @@
         <v>5</v>
       </c>
       <c r="G169" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H169" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I169" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170">
@@ -6137,13 +6137,13 @@
         <v>5</v>
       </c>
       <c r="G170" s="2" t="n">
-        <v>44946</v>
+        <v>44954</v>
       </c>
       <c r="H170" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I170" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171">
@@ -6170,13 +6170,13 @@
         <v>5</v>
       </c>
       <c r="G171" s="2" t="n">
-        <v>44944</v>
+        <v>44954</v>
       </c>
       <c r="H171" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I171" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172">
@@ -6203,13 +6203,13 @@
         <v>5</v>
       </c>
       <c r="G172" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H172" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I172" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173">
@@ -6236,13 +6236,13 @@
         <v>5</v>
       </c>
       <c r="G173" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H173" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I173" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174">
@@ -6269,13 +6269,13 @@
         <v>5</v>
       </c>
       <c r="G174" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H174" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
@@ -6302,13 +6302,13 @@
         <v>5</v>
       </c>
       <c r="G175" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H175" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I175" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176">
@@ -6335,13 +6335,13 @@
         <v>5</v>
       </c>
       <c r="G176" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H176" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I176" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -6368,13 +6368,13 @@
         <v>5</v>
       </c>
       <c r="G177" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H177" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">
@@ -6401,13 +6401,13 @@
         <v>5</v>
       </c>
       <c r="G178" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H178" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -6434,13 +6434,13 @@
         <v>5</v>
       </c>
       <c r="G179" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H179" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I179" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -6467,13 +6467,13 @@
         <v>5</v>
       </c>
       <c r="G180" s="2" t="n">
-        <v>44950</v>
+        <v>44954</v>
       </c>
       <c r="H180" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I180" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181">
@@ -6500,13 +6500,13 @@
         <v>5</v>
       </c>
       <c r="G181" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H181" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -6533,13 +6533,13 @@
         <v>5</v>
       </c>
       <c r="G182" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H182" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -6566,13 +6566,13 @@
         <v>5</v>
       </c>
       <c r="G183" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H183" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I183" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="184">
@@ -6599,13 +6599,13 @@
         <v>5</v>
       </c>
       <c r="G184" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H184" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I184" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
@@ -6632,13 +6632,13 @@
         <v>5</v>
       </c>
       <c r="G185" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H185" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I185" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186">
@@ -6665,13 +6665,13 @@
         <v>5</v>
       </c>
       <c r="G186" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H186" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I186" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187">
@@ -6698,13 +6698,13 @@
         <v>5</v>
       </c>
       <c r="G187" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H187" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I187" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -6731,13 +6731,13 @@
         <v>5</v>
       </c>
       <c r="G188" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H188" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -6764,13 +6764,13 @@
         <v>5</v>
       </c>
       <c r="G189" s="2" t="n">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="H189" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I189" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -6797,13 +6797,13 @@
         <v>5</v>
       </c>
       <c r="G190" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H190" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -6830,13 +6830,13 @@
         <v>5</v>
       </c>
       <c r="G191" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H191" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I191" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192">
@@ -6863,13 +6863,13 @@
         <v>5</v>
       </c>
       <c r="G192" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H192" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I192" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193">
@@ -6896,13 +6896,13 @@
         <v>5</v>
       </c>
       <c r="G193" s="2" t="n">
-        <v>44952</v>
+        <v>44954</v>
       </c>
       <c r="H193" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I193" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194">
@@ -6929,13 +6929,13 @@
         <v>5</v>
       </c>
       <c r="G194" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H194" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -6962,13 +6962,13 @@
         <v>5</v>
       </c>
       <c r="G195" s="2" t="n">
-        <v>44951</v>
+        <v>44954</v>
       </c>
       <c r="H195" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I195" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -6992,16 +6992,16 @@
         </is>
       </c>
       <c r="F196" t="n">
+        <v>5</v>
+      </c>
+      <c r="G196" s="2" t="n">
+        <v>44954</v>
+      </c>
+      <c r="H196" s="2" t="n">
+        <v>44954</v>
+      </c>
+      <c r="I196" t="n">
         <v>4</v>
-      </c>
-      <c r="G196" s="2" t="n">
-        <v>44953</v>
-      </c>
-      <c r="H196" s="2" t="n">
-        <v>117642</v>
-      </c>
-      <c r="I196" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -7025,10 +7025,10 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G197" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H197" s="2" t="n">
         <v>117642</v>
@@ -7058,16 +7058,16 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G198" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H198" s="2" t="n">
-        <v>117642</v>
+        <v>44954</v>
       </c>
       <c r="I198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199">
@@ -7091,10 +7091,10 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G199" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H199" s="2" t="n">
         <v>117642</v>
@@ -7124,10 +7124,10 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G200" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H200" s="2" t="n">
         <v>117642</v>
@@ -7157,10 +7157,10 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G201" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H201" s="2" t="n">
         <v>117642</v>
@@ -7190,16 +7190,16 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G202" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H202" s="2" t="n">
-        <v>117642</v>
+        <v>44954</v>
       </c>
       <c r="I202" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
@@ -7223,10 +7223,10 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G203" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H203" s="2" t="n">
         <v>117642</v>
@@ -7256,10 +7256,10 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G204" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H204" s="2" t="n">
         <v>117642</v>
@@ -7289,10 +7289,10 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G205" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H205" s="2" t="n">
         <v>117642</v>
@@ -7322,10 +7322,10 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G206" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H206" s="2" t="n">
         <v>117642</v>
@@ -7355,10 +7355,10 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G207" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H207" s="2" t="n">
         <v>117642</v>
@@ -7388,10 +7388,10 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G208" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H208" s="2" t="n">
         <v>117642</v>
@@ -7421,10 +7421,10 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G209" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H209" s="2" t="n">
         <v>117642</v>
@@ -7454,10 +7454,10 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G210" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H210" s="2" t="n">
         <v>117642</v>
@@ -7487,10 +7487,10 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G211" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H211" s="2" t="n">
         <v>117642</v>
@@ -7520,10 +7520,10 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G212" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H212" s="2" t="n">
         <v>117642</v>
@@ -7553,10 +7553,10 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G213" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H213" s="2" t="n">
         <v>117642</v>
@@ -7589,7 +7589,7 @@
         <v>3</v>
       </c>
       <c r="G214" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H214" s="2" t="n">
         <v>117642</v>
@@ -7619,16 +7619,16 @@
         </is>
       </c>
       <c r="F215" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G215" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H215" s="2" t="n">
-        <v>117642</v>
+        <v>44954</v>
       </c>
       <c r="I215" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216">
@@ -7652,10 +7652,10 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G216" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H216" s="2" t="n">
         <v>117642</v>
@@ -7685,10 +7685,10 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G217" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H217" s="2" t="n">
         <v>117642</v>
@@ -7718,10 +7718,10 @@
         </is>
       </c>
       <c r="F218" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G218" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H218" s="2" t="n">
         <v>117642</v>
@@ -7751,10 +7751,10 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G219" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H219" s="2" t="n">
         <v>117642</v>
@@ -7784,10 +7784,10 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G220" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H220" s="2" t="n">
         <v>117642</v>
@@ -7820,7 +7820,7 @@
         <v>0</v>
       </c>
       <c r="G221" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H221" s="2" t="n">
         <v>117642</v>
@@ -7850,10 +7850,10 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G222" s="2" t="n">
-        <v>44953</v>
+        <v>44954</v>
       </c>
       <c r="H222" s="2" t="n">
         <v>117642</v>

</xml_diff>

<commit_message>
update(try_again): proper instruction, vim keys, gitignore, csv files introduced
</commit_message>
<xml_diff>
--- a/capture.xlsx
+++ b/capture.xlsx
@@ -510,13 +510,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -545,13 +545,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -580,13 +580,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -615,13 +615,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -650,13 +650,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -685,13 +685,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -720,13 +720,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -755,13 +755,13 @@
         <v>5</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -790,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -825,13 +825,13 @@
         <v>5</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -860,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -895,13 +895,13 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -930,13 +930,13 @@
         <v>5</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H14" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -965,13 +965,13 @@
         <v>5</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H15" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1000,13 +1000,13 @@
         <v>5</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1035,13 +1035,13 @@
         <v>5</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H17" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1070,13 +1070,13 @@
         <v>5</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19">
@@ -1105,13 +1105,13 @@
         <v>5</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20">
@@ -1140,13 +1140,13 @@
         <v>5</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H20" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1175,13 +1175,13 @@
         <v>5</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H21" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1210,13 +1210,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H22" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1246,13 +1246,13 @@
         <v>5</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H23" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1281,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H24" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1316,13 +1316,13 @@
         <v>5</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H25" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26">
@@ -1351,13 +1351,13 @@
         <v>5</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H26" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1386,13 +1386,13 @@
         <v>5</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H27" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1421,13 +1421,13 @@
         <v>5</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1456,13 +1456,13 @@
         <v>5</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H29" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1491,13 +1491,13 @@
         <v>5</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H30" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1526,13 +1526,13 @@
         <v>5</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H31" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1561,13 +1561,13 @@
         <v>5</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1596,13 +1596,13 @@
         <v>5</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H33" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1631,13 +1631,13 @@
         <v>5</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1666,13 +1666,13 @@
         <v>5</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H35" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1701,13 +1701,13 @@
         <v>5</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H36" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1736,13 +1736,13 @@
         <v>5</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H37" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38">
@@ -1771,13 +1771,13 @@
         <v>5</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H38" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1806,13 +1806,13 @@
         <v>5</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H39" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1841,13 +1841,13 @@
         <v>5</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H40" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1876,13 +1876,13 @@
         <v>5</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H41" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1911,13 +1911,13 @@
         <v>5</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H42" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1944,13 +1944,13 @@
         <v>5</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H43" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -1977,13 +1977,13 @@
         <v>5</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H44" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -2010,13 +2010,13 @@
         <v>5</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H45" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2043,13 +2043,13 @@
         <v>5</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H46" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2076,13 +2076,13 @@
         <v>5</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H47" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2109,13 +2109,13 @@
         <v>5</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H48" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -2142,13 +2142,13 @@
         <v>5</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H49" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2175,13 +2175,13 @@
         <v>5</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H50" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I50" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2208,13 +2208,13 @@
         <v>5</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H51" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2241,13 +2241,13 @@
         <v>5</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H52" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2274,13 +2274,13 @@
         <v>5</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H53" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="54">
@@ -2307,13 +2307,13 @@
         <v>5</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H54" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I54" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -2340,13 +2340,13 @@
         <v>5</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H55" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2373,13 +2373,13 @@
         <v>5</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H56" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2406,13 +2406,13 @@
         <v>5</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H57" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I57" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -2439,13 +2439,13 @@
         <v>5</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H58" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2472,13 +2472,13 @@
         <v>5</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H59" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2505,13 +2505,13 @@
         <v>5</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H60" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -2538,13 +2538,13 @@
         <v>5</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H61" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I61" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2571,13 +2571,13 @@
         <v>5</v>
       </c>
       <c r="G62" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H62" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I62" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -2604,13 +2604,13 @@
         <v>5</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H63" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I63" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2637,13 +2637,13 @@
         <v>5</v>
       </c>
       <c r="G64" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H64" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2670,13 +2670,13 @@
         <v>5</v>
       </c>
       <c r="G65" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H65" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2703,13 +2703,13 @@
         <v>5</v>
       </c>
       <c r="G66" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H66" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2736,13 +2736,13 @@
         <v>5</v>
       </c>
       <c r="G67" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H67" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2769,13 +2769,13 @@
         <v>5</v>
       </c>
       <c r="G68" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H68" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I68" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2802,13 +2802,13 @@
         <v>5</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H69" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I69" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -2835,13 +2835,13 @@
         <v>5</v>
       </c>
       <c r="G70" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H70" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2868,13 +2868,13 @@
         <v>5</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H71" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I71" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -2901,13 +2901,13 @@
         <v>5</v>
       </c>
       <c r="G72" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H72" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="73">
@@ -2934,13 +2934,13 @@
         <v>5</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H73" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I73" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2967,13 +2967,13 @@
         <v>5</v>
       </c>
       <c r="G74" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H74" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I74" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -3000,13 +3000,13 @@
         <v>5</v>
       </c>
       <c r="G75" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H75" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I75" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -3033,13 +3033,13 @@
         <v>5</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H76" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -3066,13 +3066,13 @@
         <v>5</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H77" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I77" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="78">
@@ -3099,13 +3099,13 @@
         <v>5</v>
       </c>
       <c r="G78" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H78" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I78" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -3132,13 +3132,13 @@
         <v>5</v>
       </c>
       <c r="G79" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H79" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3165,13 +3165,13 @@
         <v>5</v>
       </c>
       <c r="G80" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H80" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -3198,13 +3198,13 @@
         <v>5</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H81" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="82">
@@ -3231,13 +3231,13 @@
         <v>5</v>
       </c>
       <c r="G82" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H82" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -3264,13 +3264,13 @@
         <v>5</v>
       </c>
       <c r="G83" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H83" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3297,13 +3297,13 @@
         <v>5</v>
       </c>
       <c r="G84" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H84" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3331,13 +3331,13 @@
         <v>5</v>
       </c>
       <c r="G85" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H85" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I85" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -3364,13 +3364,13 @@
         <v>5</v>
       </c>
       <c r="G86" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H86" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I86" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="87">
@@ -3397,13 +3397,13 @@
         <v>5</v>
       </c>
       <c r="G87" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H87" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I87" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="88">
@@ -3430,13 +3430,13 @@
         <v>5</v>
       </c>
       <c r="G88" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H88" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I88" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="89">
@@ -3463,13 +3463,13 @@
         <v>5</v>
       </c>
       <c r="G89" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H89" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I89" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3496,13 +3496,13 @@
         <v>5</v>
       </c>
       <c r="G90" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H90" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I90" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -3529,13 +3529,13 @@
         <v>5</v>
       </c>
       <c r="G91" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H91" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3562,13 +3562,13 @@
         <v>5</v>
       </c>
       <c r="G92" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H92" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I92" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -3595,13 +3595,13 @@
         <v>5</v>
       </c>
       <c r="G93" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H93" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I93" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -3628,13 +3628,13 @@
         <v>5</v>
       </c>
       <c r="G94" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H94" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I94" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -3661,13 +3661,13 @@
         <v>5</v>
       </c>
       <c r="G95" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H95" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I95" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3694,13 +3694,13 @@
         <v>5</v>
       </c>
       <c r="G96" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H96" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I96" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
@@ -3727,13 +3727,13 @@
         <v>5</v>
       </c>
       <c r="G97" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H97" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3760,13 +3760,13 @@
         <v>5</v>
       </c>
       <c r="G98" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H98" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I98" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -3793,13 +3793,13 @@
         <v>5</v>
       </c>
       <c r="G99" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H99" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3826,13 +3826,13 @@
         <v>5</v>
       </c>
       <c r="G100" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H100" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3859,13 +3859,13 @@
         <v>5</v>
       </c>
       <c r="G101" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H101" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I101" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -3892,13 +3892,13 @@
         <v>5</v>
       </c>
       <c r="G102" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H102" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="103">
@@ -3925,13 +3925,13 @@
         <v>5</v>
       </c>
       <c r="G103" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H103" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -3958,13 +3958,13 @@
         <v>5</v>
       </c>
       <c r="G104" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H104" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I104" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -3991,13 +3991,13 @@
         <v>5</v>
       </c>
       <c r="G105" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H105" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I105" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -4024,13 +4024,13 @@
         <v>5</v>
       </c>
       <c r="G106" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H106" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -4057,13 +4057,13 @@
         <v>5</v>
       </c>
       <c r="G107" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H107" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I107" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
@@ -4090,13 +4090,13 @@
         <v>5</v>
       </c>
       <c r="G108" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H108" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I108" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4123,13 +4123,13 @@
         <v>5</v>
       </c>
       <c r="G109" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H109" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I109" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -4156,13 +4156,13 @@
         <v>5</v>
       </c>
       <c r="G110" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H110" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I110" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -4189,13 +4189,13 @@
         <v>5</v>
       </c>
       <c r="G111" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H111" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -4222,13 +4222,13 @@
         <v>5</v>
       </c>
       <c r="G112" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H112" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I112" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -4255,13 +4255,13 @@
         <v>5</v>
       </c>
       <c r="G113" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H113" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -4288,13 +4288,13 @@
         <v>5</v>
       </c>
       <c r="G114" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H114" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I114" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -4321,13 +4321,13 @@
         <v>5</v>
       </c>
       <c r="G115" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H115" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I115" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -4354,13 +4354,13 @@
         <v>5</v>
       </c>
       <c r="G116" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H116" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I116" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -4387,13 +4387,13 @@
         <v>5</v>
       </c>
       <c r="G117" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H117" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I117" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
@@ -4420,13 +4420,13 @@
         <v>5</v>
       </c>
       <c r="G118" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H118" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I118" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="119">
@@ -4453,13 +4453,13 @@
         <v>5</v>
       </c>
       <c r="G119" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H119" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I119" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -4486,13 +4486,13 @@
         <v>5</v>
       </c>
       <c r="G120" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H120" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I120" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -4519,13 +4519,13 @@
         <v>5</v>
       </c>
       <c r="G121" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H121" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I121" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -4552,13 +4552,13 @@
         <v>5</v>
       </c>
       <c r="G122" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H122" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I122" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
@@ -4585,13 +4585,13 @@
         <v>5</v>
       </c>
       <c r="G123" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H123" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I123" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="124">
@@ -4618,13 +4618,13 @@
         <v>5</v>
       </c>
       <c r="G124" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H124" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I124" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -4651,13 +4651,13 @@
         <v>5</v>
       </c>
       <c r="G125" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H125" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I125" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
@@ -4684,13 +4684,13 @@
         <v>5</v>
       </c>
       <c r="G126" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H126" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I126" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
@@ -4717,13 +4717,13 @@
         <v>5</v>
       </c>
       <c r="G127" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H127" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -4750,13 +4750,13 @@
         <v>5</v>
       </c>
       <c r="G128" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H128" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I128" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
@@ -4783,13 +4783,13 @@
         <v>5</v>
       </c>
       <c r="G129" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H129" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I129" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -4816,13 +4816,13 @@
         <v>5</v>
       </c>
       <c r="G130" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H130" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I130" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131">
@@ -4849,13 +4849,13 @@
         <v>5</v>
       </c>
       <c r="G131" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H131" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -4882,13 +4882,13 @@
         <v>5</v>
       </c>
       <c r="G132" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H132" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I132" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -4915,13 +4915,13 @@
         <v>5</v>
       </c>
       <c r="G133" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H133" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I133" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -4948,13 +4948,13 @@
         <v>5</v>
       </c>
       <c r="G134" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H134" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -4981,13 +4981,13 @@
         <v>5</v>
       </c>
       <c r="G135" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H135" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I135" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -5014,13 +5014,13 @@
         <v>5</v>
       </c>
       <c r="G136" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H136" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I136" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -5047,13 +5047,13 @@
         <v>5</v>
       </c>
       <c r="G137" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H137" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I137" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="138">
@@ -5080,13 +5080,13 @@
         <v>5</v>
       </c>
       <c r="G138" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H138" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I138" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -5113,13 +5113,13 @@
         <v>5</v>
       </c>
       <c r="G139" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H139" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I139" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140">
@@ -5146,13 +5146,13 @@
         <v>5</v>
       </c>
       <c r="G140" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H140" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I140" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
@@ -5179,13 +5179,13 @@
         <v>5</v>
       </c>
       <c r="G141" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H141" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I141" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -5212,13 +5212,13 @@
         <v>5</v>
       </c>
       <c r="G142" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H142" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I142" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -5245,13 +5245,13 @@
         <v>5</v>
       </c>
       <c r="G143" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H143" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I143" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -5278,13 +5278,13 @@
         <v>5</v>
       </c>
       <c r="G144" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H144" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I144" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="145">
@@ -5311,13 +5311,13 @@
         <v>5</v>
       </c>
       <c r="G145" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H145" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I145" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -5344,13 +5344,13 @@
         <v>5</v>
       </c>
       <c r="G146" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H146" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I146" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="147">
@@ -5377,13 +5377,13 @@
         <v>5</v>
       </c>
       <c r="G147" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H147" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -5410,13 +5410,13 @@
         <v>5</v>
       </c>
       <c r="G148" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H148" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I148" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -5443,13 +5443,13 @@
         <v>5</v>
       </c>
       <c r="G149" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H149" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -5476,13 +5476,13 @@
         <v>5</v>
       </c>
       <c r="G150" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H150" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I150" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="151">
@@ -5509,13 +5509,13 @@
         <v>5</v>
       </c>
       <c r="G151" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H151" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I151" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="152">
@@ -5542,13 +5542,13 @@
         <v>5</v>
       </c>
       <c r="G152" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H152" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I152" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -5575,13 +5575,13 @@
         <v>5</v>
       </c>
       <c r="G153" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H153" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I153" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -5608,13 +5608,13 @@
         <v>5</v>
       </c>
       <c r="G154" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H154" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I154" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -5641,13 +5641,13 @@
         <v>5</v>
       </c>
       <c r="G155" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H155" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I155" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -5675,13 +5675,13 @@
         <v>5</v>
       </c>
       <c r="G156" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H156" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I156" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="157">
@@ -5708,13 +5708,13 @@
         <v>5</v>
       </c>
       <c r="G157" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H157" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I157" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -5741,13 +5741,13 @@
         <v>5</v>
       </c>
       <c r="G158" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H158" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I158" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -5774,13 +5774,13 @@
         <v>5</v>
       </c>
       <c r="G159" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H159" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I159" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="160">
@@ -5807,13 +5807,13 @@
         <v>5</v>
       </c>
       <c r="G160" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H160" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I160" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161">
@@ -5840,13 +5840,13 @@
         <v>5</v>
       </c>
       <c r="G161" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H161" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I161" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -5873,13 +5873,13 @@
         <v>5</v>
       </c>
       <c r="G162" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H162" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I162" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -5906,13 +5906,13 @@
         <v>5</v>
       </c>
       <c r="G163" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H163" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I163" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -5939,13 +5939,13 @@
         <v>5</v>
       </c>
       <c r="G164" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H164" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I164" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -5972,13 +5972,13 @@
         <v>5</v>
       </c>
       <c r="G165" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H165" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I165" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -6005,13 +6005,13 @@
         <v>5</v>
       </c>
       <c r="G166" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H166" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -6038,13 +6038,13 @@
         <v>5</v>
       </c>
       <c r="G167" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H167" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -6071,13 +6071,13 @@
         <v>5</v>
       </c>
       <c r="G168" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H168" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I168" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -6104,13 +6104,13 @@
         <v>5</v>
       </c>
       <c r="G169" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H169" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I169" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -6137,13 +6137,13 @@
         <v>5</v>
       </c>
       <c r="G170" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H170" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I170" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -6170,13 +6170,13 @@
         <v>5</v>
       </c>
       <c r="G171" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H171" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I171" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -6203,13 +6203,13 @@
         <v>5</v>
       </c>
       <c r="G172" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H172" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I172" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -6236,13 +6236,13 @@
         <v>5</v>
       </c>
       <c r="G173" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H173" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I173" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174">
@@ -6269,13 +6269,13 @@
         <v>5</v>
       </c>
       <c r="G174" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H174" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I174" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -6302,13 +6302,13 @@
         <v>5</v>
       </c>
       <c r="G175" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H175" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I175" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176">
@@ -6335,13 +6335,13 @@
         <v>5</v>
       </c>
       <c r="G176" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H176" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I176" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -6368,13 +6368,13 @@
         <v>5</v>
       </c>
       <c r="G177" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H177" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I177" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="178">
@@ -6401,13 +6401,13 @@
         <v>5</v>
       </c>
       <c r="G178" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H178" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -6434,13 +6434,13 @@
         <v>5</v>
       </c>
       <c r="G179" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H179" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I179" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -6467,13 +6467,13 @@
         <v>5</v>
       </c>
       <c r="G180" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H180" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I180" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -6500,13 +6500,13 @@
         <v>5</v>
       </c>
       <c r="G181" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H181" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -6533,13 +6533,13 @@
         <v>5</v>
       </c>
       <c r="G182" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H182" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -6566,13 +6566,13 @@
         <v>5</v>
       </c>
       <c r="G183" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H183" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I183" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
@@ -6599,13 +6599,13 @@
         <v>5</v>
       </c>
       <c r="G184" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H184" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I184" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -6632,13 +6632,13 @@
         <v>5</v>
       </c>
       <c r="G185" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H185" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I185" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186">
@@ -6665,13 +6665,13 @@
         <v>5</v>
       </c>
       <c r="G186" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H186" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I186" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -6698,13 +6698,13 @@
         <v>5</v>
       </c>
       <c r="G187" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H187" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I187" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -6731,13 +6731,13 @@
         <v>5</v>
       </c>
       <c r="G188" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H188" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -6764,13 +6764,13 @@
         <v>5</v>
       </c>
       <c r="G189" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H189" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I189" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -6797,13 +6797,13 @@
         <v>5</v>
       </c>
       <c r="G190" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H190" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I190" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="191">
@@ -6830,13 +6830,13 @@
         <v>5</v>
       </c>
       <c r="G191" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H191" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I191" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192">
@@ -6863,13 +6863,13 @@
         <v>5</v>
       </c>
       <c r="G192" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H192" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I192" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -6896,13 +6896,13 @@
         <v>5</v>
       </c>
       <c r="G193" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H193" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I193" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194">
@@ -6929,13 +6929,13 @@
         <v>5</v>
       </c>
       <c r="G194" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H194" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -6962,13 +6962,13 @@
         <v>5</v>
       </c>
       <c r="G195" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H195" s="2" t="n">
         <v>117642</v>
       </c>
       <c r="I195" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196">
@@ -6995,13 +6995,13 @@
         <v>5</v>
       </c>
       <c r="G196" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H196" s="2" t="n">
         <v>44954</v>
       </c>
       <c r="I196" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
@@ -7061,13 +7061,13 @@
         <v>5</v>
       </c>
       <c r="G198" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H198" s="2" t="n">
         <v>44954</v>
       </c>
       <c r="I198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -7193,13 +7193,13 @@
         <v>5</v>
       </c>
       <c r="G202" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H202" s="2" t="n">
         <v>44954</v>
       </c>
       <c r="I202" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -7622,13 +7622,13 @@
         <v>5</v>
       </c>
       <c r="G215" s="2" t="n">
-        <v>44954</v>
+        <v>45435</v>
       </c>
       <c r="H215" s="2" t="n">
         <v>44954</v>
       </c>
       <c r="I215" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">

</xml_diff>